<commit_message>
Created CBLs and revised BPS
</commit_message>
<xml_diff>
--- a/seed/tests/data/building-performance-standards-sample-2021.xlsx
+++ b/seed/tests/data/building-performance-standards-sample-2021.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/achapin/seed/seed/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A73213F-07CC-A242-8F11-77D6E018211E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4C6C3EF-B56D-DF4D-9FE1-227CF59B5C68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-1420" yWindow="1040" windowWidth="38400" windowHeight="20180" xr2:uid="{ABA70866-58E3-E741-9E6E-8CBE8BD4F008}"/>
+    <workbookView xWindow="0" yWindow="1040" windowWidth="35840" windowHeight="20180" xr2:uid="{ABA70866-58E3-E741-9E6E-8CBE8BD4F008}"/>
   </bookViews>
   <sheets>
     <sheet name="BPS Data" sheetId="2" r:id="rId1"/>
@@ -305,162 +305,7 @@
     <cellStyle name="Normal 2" xfId="1" xr:uid="{4367F287-F053-B14B-BB78-7F2A1A8270CC}"/>
     <cellStyle name="Normal 3" xfId="2" xr:uid="{FC32E4A8-5101-754C-BA01-BA4BA25B0A66}"/>
   </cellStyles>
-  <dxfs count="22">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -773,7 +618,7 @@
   <dimension ref="A1:Q10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P8" sqref="P8"/>
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -881,10 +726,10 @@
         <v>44561</v>
       </c>
       <c r="P2">
-        <v>99</v>
+        <v>81</v>
       </c>
       <c r="Q2">
-        <v>2021</v>
+        <v>2022</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
@@ -934,10 +779,10 @@
         <v>44561</v>
       </c>
       <c r="P3">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="Q3">
-        <v>2021</v>
+        <v>2022</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
@@ -987,10 +832,10 @@
         <v>44561</v>
       </c>
       <c r="P4">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="Q4">
-        <v>2021</v>
+        <v>2022</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
@@ -1040,10 +885,10 @@
         <v>44561</v>
       </c>
       <c r="P5">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="Q5">
-        <v>2021</v>
+        <v>2022</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
@@ -1093,10 +938,10 @@
         <v>44561</v>
       </c>
       <c r="P6">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="Q6">
-        <v>2021</v>
+        <v>2022</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
@@ -1146,10 +991,10 @@
         <v>44561</v>
       </c>
       <c r="P7">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="Q7">
-        <v>2021</v>
+        <v>2022</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
@@ -1199,10 +1044,10 @@
         <v>44561</v>
       </c>
       <c r="P8">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="Q8">
-        <v>2021</v>
+        <v>2022</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
@@ -1252,10 +1097,10 @@
         <v>44561</v>
       </c>
       <c r="P9">
-        <v>113</v>
+        <v>100</v>
       </c>
       <c r="Q9">
-        <v>2021</v>
+        <v>2022</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
@@ -1303,10 +1148,10 @@
         <v>44561</v>
       </c>
       <c r="P10">
-        <v>150</v>
+        <v>121</v>
       </c>
       <c r="Q10">
-        <v>2021</v>
+        <v>2022</v>
       </c>
     </row>
   </sheetData>

</xml_diff>